<commit_message>
Synchronized branch with changes from trunk by merging in r56-63.
</commit_message>
<xml_diff>
--- a/branches/serialization-refactor/Documentation/Turn Files/Turn File Contents.xlsx
+++ b/branches/serialization-refactor/Documentation/Turn Files/Turn File Contents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>ConsoleState</t>
   </si>
@@ -258,7 +258,13 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>RaceData (not a RaceData object)</t>
+    <t>PlayerRace</t>
+  </si>
+  <si>
+    <t>BattlePlans (in PlayerData)</t>
+  </si>
+  <si>
+    <t>PlayerRelations (in PlayerData)</t>
   </si>
 </sst>
 </file>
@@ -310,11 +316,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,10 +1095,7 @@
         <v>67</v>
       </c>
       <c r="K32" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1116,10 +1120,7 @@
         <v>67</v>
       </c>
       <c r="K34" t="s">
-        <v>44</v>
-      </c>
-      <c r="L34" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1179,8 +1180,11 @@
       <c r="D39" t="s">
         <v>80</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>52</v>
+      <c r="K39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1271,6 +1275,9 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
+        <v>66</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>66</v>
       </c>
       <c r="L47" t="s">

</xml_diff>